<commit_message>
ec and bug fix for rst packets
</commit_message>
<xml_diff>
--- a/proj3/EC Data.xlsx
+++ b/proj3/EC Data.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Proj 3a" sheetId="1" r:id="rId1"/>
+    <sheet name="Proj 3b" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>time elapsed: 30minute(s)</t>
   </si>
@@ -234,6 +235,42 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>&lt; 1KB</t>
+  </si>
+  <si>
+    <t>1-2KB</t>
+  </si>
+  <si>
+    <t>2-4KB</t>
+  </si>
+  <si>
+    <t>4-8KB</t>
+  </si>
+  <si>
+    <t>8-16KB</t>
+  </si>
+  <si>
+    <t>16-32KB</t>
+  </si>
+  <si>
+    <t>32-64KB</t>
+  </si>
+  <si>
+    <t>64-128KB</t>
+  </si>
+  <si>
+    <t>128-256KB</t>
+  </si>
+  <si>
+    <t>256-512KB</t>
+  </si>
+  <si>
+    <t>512-1024KB</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -242,7 +279,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -309,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -373,7 +410,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -395,7 +431,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$6</c:f>
+              <c:f>'Proj 3a'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -417,7 +453,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7</c:f>
+              <c:f>'Proj 3a'!$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -433,7 +469,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
+              <c:f>'Proj 3a'!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -455,7 +491,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$7</c:f>
+              <c:f>'Proj 3a'!$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -471,7 +507,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$6</c:f>
+              <c:f>'Proj 3a'!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -493,7 +529,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7</c:f>
+              <c:f>'Proj 3a'!$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -509,7 +545,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$6</c:f>
+              <c:f>'Proj 3a'!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -531,7 +567,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$7</c:f>
+              <c:f>'Proj 3a'!$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -547,7 +583,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$6</c:f>
+              <c:f>'Proj 3a'!$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -569,7 +605,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$7</c:f>
+              <c:f>'Proj 3a'!$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -585,7 +621,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$6</c:f>
+              <c:f>'Proj 3a'!$G$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -607,7 +643,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$7</c:f>
+              <c:f>'Proj 3a'!$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -623,7 +659,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$6</c:f>
+              <c:f>'Proj 3a'!$H$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -647,7 +683,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$7</c:f>
+              <c:f>'Proj 3a'!$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -663,7 +699,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$6</c:f>
+              <c:f>'Proj 3a'!$I$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -687,7 +723,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$7</c:f>
+              <c:f>'Proj 3a'!$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -703,7 +739,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$6</c:f>
+              <c:f>'Proj 3a'!$J$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -727,7 +763,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$7</c:f>
+              <c:f>'Proj 3a'!$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -743,7 +779,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$6</c:f>
+              <c:f>'Proj 3a'!$K$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -767,7 +803,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$7</c:f>
+              <c:f>'Proj 3a'!$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -783,7 +819,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$6</c:f>
+              <c:f>'Proj 3a'!$L$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -807,7 +843,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$7</c:f>
+              <c:f>'Proj 3a'!$L$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -823,7 +859,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$6</c:f>
+              <c:f>'Proj 3a'!$M$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -847,7 +883,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$7</c:f>
+              <c:f>'Proj 3a'!$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -863,7 +899,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$6</c:f>
+              <c:f>'Proj 3a'!$N$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -888,7 +924,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$7</c:f>
+              <c:f>'Proj 3a'!$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -904,7 +940,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$6</c:f>
+              <c:f>'Proj 3a'!$O$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -929,7 +965,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$7</c:f>
+              <c:f>'Proj 3a'!$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -945,7 +981,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$6</c:f>
+              <c:f>'Proj 3a'!$P$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -970,7 +1006,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$7</c:f>
+              <c:f>'Proj 3a'!$P$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -986,7 +1022,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$6</c:f>
+              <c:f>'Proj 3a'!$Q$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1011,7 +1047,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$7</c:f>
+              <c:f>'Proj 3a'!$Q$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1027,7 +1063,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$6</c:f>
+              <c:f>'Proj 3a'!$R$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1052,7 +1088,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$7</c:f>
+              <c:f>'Proj 3a'!$R$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1068,7 +1104,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$6</c:f>
+              <c:f>'Proj 3a'!$S$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1093,7 +1129,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$7</c:f>
+              <c:f>'Proj 3a'!$S$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1109,7 +1145,7 @@
           <c:order val="18"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$6</c:f>
+              <c:f>'Proj 3a'!$T$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1133,7 +1169,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$7</c:f>
+              <c:f>'Proj 3a'!$T$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1149,7 +1185,7 @@
           <c:order val="19"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$6</c:f>
+              <c:f>'Proj 3a'!$U$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1173,7 +1209,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$7</c:f>
+              <c:f>'Proj 3a'!$U$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1189,7 +1225,7 @@
           <c:order val="20"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$6</c:f>
+              <c:f>'Proj 3a'!$V$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1213,7 +1249,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$7</c:f>
+              <c:f>'Proj 3a'!$V$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1229,7 +1265,7 @@
           <c:order val="21"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$W$6</c:f>
+              <c:f>'Proj 3a'!$W$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1253,7 +1289,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$7</c:f>
+              <c:f>'Proj 3a'!$W$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1269,7 +1305,7 @@
           <c:order val="22"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$6</c:f>
+              <c:f>'Proj 3a'!$X$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1293,7 +1329,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$X$7</c:f>
+              <c:f>'Proj 3a'!$X$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1309,7 +1345,7 @@
           <c:order val="23"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$6</c:f>
+              <c:f>'Proj 3a'!$Y$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1333,7 +1369,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Y$7</c:f>
+              <c:f>'Proj 3a'!$Y$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1349,7 +1385,7 @@
           <c:order val="24"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Z$6</c:f>
+              <c:f>'Proj 3a'!$Z$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1374,7 +1410,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$7</c:f>
+              <c:f>'Proj 3a'!$Z$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1390,7 +1426,7 @@
           <c:order val="25"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AA$6</c:f>
+              <c:f>'Proj 3a'!$AA$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1415,7 +1451,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AA$7</c:f>
+              <c:f>'Proj 3a'!$AA$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1431,7 +1467,7 @@
           <c:order val="26"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AB$6</c:f>
+              <c:f>'Proj 3a'!$AB$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1456,7 +1492,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AB$7</c:f>
+              <c:f>'Proj 3a'!$AB$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1472,7 +1508,7 @@
           <c:order val="27"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AC$6</c:f>
+              <c:f>'Proj 3a'!$AC$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1497,7 +1533,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AC$7</c:f>
+              <c:f>'Proj 3a'!$AC$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1513,7 +1549,7 @@
           <c:order val="28"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AD$6</c:f>
+              <c:f>'Proj 3a'!$AD$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1538,7 +1574,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AD$7</c:f>
+              <c:f>'Proj 3a'!$AD$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1554,7 +1590,7 @@
           <c:order val="29"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AE$6</c:f>
+              <c:f>'Proj 3a'!$AE$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1579,7 +1615,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AE$7</c:f>
+              <c:f>'Proj 3a'!$AE$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1599,11 +1635,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="970676144"/>
-        <c:axId val="970675056"/>
+        <c:axId val="-812255328"/>
+        <c:axId val="-812263488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="970676144"/>
+        <c:axId val="-812255328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1649,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="970675056"/>
+        <c:crossAx val="-812263488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1621,7 +1657,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="970675056"/>
+        <c:axId val="-812263488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1693,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1691,7 +1726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="970676144"/>
+        <c:crossAx val="-812255328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1706,7 +1741,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1835,7 +1869,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$21</c:f>
+              <c:f>'Proj 3a'!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1860,7 +1894,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$B$22:$F$22</c:f>
+                <c:f>'Proj 3a'!$B$22:$F$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1884,7 +1918,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$B$22:$F$22</c:f>
+                <c:f>'Proj 3a'!$B$22:$F$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1922,7 +1956,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$F$20</c:f>
+              <c:f>'Proj 3a'!$B$20:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1946,7 +1980,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$F$21</c:f>
+              <c:f>'Proj 3a'!$B$21:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1979,11 +2013,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="970679952"/>
-        <c:axId val="970682128"/>
+        <c:axId val="-812265120"/>
+        <c:axId val="-812261856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="970679952"/>
+        <c:axId val="-812265120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2062,7 +2096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="970682128"/>
+        <c:crossAx val="-812261856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2070,7 +2104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="970682128"/>
+        <c:axId val="-812261856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2161,7 +2195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="970679952"/>
+        <c:crossAx val="-812265120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2208,6 +2242,1002 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HTTP Object Size Distribution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Proj 3b'!$A$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>&lt; 1KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1-2KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2-4KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-8KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8-16KB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16-32KB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32-64KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64-128KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128-256KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256-512KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512-1024KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Proj 3b'!$A$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2287</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1876</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>138</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="-729605504"/>
+        <c:axId val="-729604960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-729605504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>SIZE (KB)</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-729604960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-729604960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> oF Packets</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-729605504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2267,6 +3297,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714374</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2579,8 +3644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3121,4 +4186,103 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="11" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>769</v>
+      </c>
+      <c r="B2">
+        <v>1987</v>
+      </c>
+      <c r="C2">
+        <v>984</v>
+      </c>
+      <c r="D2">
+        <v>1350</v>
+      </c>
+      <c r="E2">
+        <v>2287</v>
+      </c>
+      <c r="F2">
+        <v>1876</v>
+      </c>
+      <c r="G2">
+        <v>1773</v>
+      </c>
+      <c r="H2">
+        <v>1128</v>
+      </c>
+      <c r="I2">
+        <v>695</v>
+      </c>
+      <c r="J2">
+        <v>126</v>
+      </c>
+      <c r="K2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4">
+        <f>SUM(A2:K2)</f>
+        <v>13113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>